<commit_message>
Contributions update Q2 2021 second revision
</commit_message>
<xml_diff>
--- a/results/08-2021/08-2021_comparison_deflators.xlsx
+++ b/results/08-2021/08-2021_comparison_deflators.xlsx
@@ -647,10 +647,10 @@
         <v>0.0149</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.026</v>
+        <v>-0.0314</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4517</v>
+        <v>0.4518</v>
       </c>
       <c r="F5" t="n">
         <v>-0.0291</v>
@@ -659,10 +659,10 @@
         <v>-0.0331</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0847</v>
+        <v>-0.0846</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0525</v>
+        <v>-0.0524</v>
       </c>
       <c r="J5" t="n">
         <v>0.0224</v>
@@ -671,7 +671,7 @@
         <v>-0.3977</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1382</v>
+        <v>-0.1381</v>
       </c>
       <c r="M5" t="n">
         <v>-0.0277</v>
@@ -688,34 +688,34 @@
         <v>-0.0156</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0004</v>
+        <v>-0.0211</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0035</v>
+        <v>-0.0166</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0522</v>
+        <v>-0.0518</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0497</v>
+        <v>-0.0493</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0557</v>
+        <v>-0.0553</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0407</v>
+        <v>-0.0403</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0729</v>
+        <v>-0.0726</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0686</v>
+        <v>-0.0683</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0433</v>
+        <v>-0.0429</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0351</v>
+        <v>-0.0348</v>
       </c>
     </row>
     <row r="7">
@@ -729,34 +729,34 @@
         <v>-0.2564</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0407</v>
+        <v>-0.0357</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0381</v>
+        <v>-0.0373</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0571</v>
+        <v>0.1199</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1595</v>
+        <v>0.2176</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.1174</v>
+        <v>-0.0736</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.1516</v>
+        <v>-0.1049</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1467</v>
+        <v>-0.1597</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.1707</v>
+        <v>-0.1803</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0453</v>
+        <v>0.044</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1274</v>
+        <v>0.1279</v>
       </c>
     </row>
     <row r="8">
@@ -770,34 +770,34 @@
         <v>-0.2688</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0635</v>
+        <v>-0.1929</v>
       </c>
       <c r="E8" t="n">
-        <v>0.083</v>
+        <v>-0.1674</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0019</v>
+        <v>-0.1227</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2729</v>
+        <v>-0.396</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.1804</v>
+        <v>-0.3017</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.0815</v>
+        <v>-0.2013</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0408</v>
+        <v>-0.0776</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0829</v>
+        <v>-0.0344</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0159</v>
+        <v>-0.0176</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0031</v>
+        <v>0.0018</v>
       </c>
     </row>
     <row r="9">
@@ -1016,31 +1016,31 @@
         <v>0.1723</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.3335</v>
+        <v>-0.339</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.1773</v>
+        <v>-1.1764</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.019</v>
+        <v>-1.0187</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.5082</v>
+        <v>-1.5079</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.1892</v>
+        <v>-1.1877</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.5195</v>
+        <v>-0.5185</v>
       </c>
       <c r="J14" t="n">
         <v>-0.4056</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.341</v>
+        <v>-0.3408</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.2509</v>
+        <v>-0.2499</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1057,34 +1057,34 @@
         <v>-2.8281</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.6188</v>
+        <v>-1.8671</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.7327</v>
+        <v>-2.922</v>
       </c>
       <c r="F15" t="n">
-        <v>-2.1039</v>
+        <v>-2.1494</v>
       </c>
       <c r="G15" t="n">
-        <v>-3.6052</v>
+        <v>-3.6555</v>
       </c>
       <c r="H15" t="n">
-        <v>-2.0284</v>
+        <v>-2.1715</v>
       </c>
       <c r="I15" t="n">
-        <v>-1.6774</v>
+        <v>-1.8151</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.6412</v>
+        <v>-1.7742</v>
       </c>
       <c r="K15" t="n">
-        <v>-2.7388</v>
+        <v>-2.866</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.2639</v>
+        <v>-1.2664</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.4866</v>
+        <v>-0.4869</v>
       </c>
     </row>
     <row r="16">
@@ -1303,31 +1303,31 @@
         <v>-0.709</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3837</v>
+        <v>0.3351</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.013</v>
+        <v>-0.0136</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3314</v>
+        <v>0.331</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0588</v>
+        <v>0.0586</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.0481</v>
+        <v>-0.0482</v>
       </c>
       <c r="I21" t="n">
         <v>-0.2135</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.2684</v>
+        <v>-0.2683</v>
       </c>
       <c r="K21" t="n">
         <v>0.183</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.0563</v>
+        <v>-0.0562</v>
       </c>
       <c r="M21" t="n">
         <v>-0.1339</v>
@@ -1385,34 +1385,34 @@
         <v>0.2168</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.1167</v>
+        <v>-0.0246</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0462</v>
+        <v>0.1351</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.0219</v>
+        <v>-0.0017</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.1148</v>
+        <v>-0.0963</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1907</v>
+        <v>0.1275</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1859</v>
+        <v>0.124</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1993</v>
+        <v>0.2015</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1864</v>
+        <v>0.1896</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.0168</v>
+        <v>-0.0175</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0081</v>
+        <v>0.0083</v>
       </c>
     </row>
     <row r="24">
@@ -1426,34 +1426,34 @@
         <v>-0.1693</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.2187</v>
+        <v>-0.2279</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.1731</v>
+        <v>-0.182</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.1493</v>
+        <v>-0.1537</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.2066</v>
+        <v>-0.211</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.1615</v>
+        <v>-0.1659</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.1664</v>
+        <v>-0.1707</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.1372</v>
+        <v>-0.1414</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0634</v>
+        <v>-0.0676</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.0315</v>
+        <v>-0.0316</v>
       </c>
       <c r="M24" t="n">
-        <v>-0.0191</v>
+        <v>-0.0192</v>
       </c>
     </row>
     <row r="25">
@@ -1590,16 +1590,16 @@
         <v>-0.2283</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.2053</v>
+        <v>-0.2049</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.057</v>
+        <v>-0.0568</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.099</v>
+        <v>-0.0988</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.2137</v>
+        <v>-0.2135</v>
       </c>
       <c r="H28" t="n">
         <v>-0.0711</v>
@@ -1754,7 +1754,7 @@
         <v>-0.0107</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0053</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1766,10 +1766,10 @@
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -1795,34 +1795,34 @@
         <v>-0.0202</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0002</v>
+        <v>-0.0205</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0002</v>
+        <v>-0.02</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0002</v>
+        <v>0.0006</v>
       </c>
     </row>
     <row r="34">
@@ -1836,34 +1836,34 @@
         <v>-0.0008</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0008</v>
+        <v>0.0042</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.0008</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.0008</v>
+        <v>0.0621</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>0.0581</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>0.0438</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>0.0468</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>-0.013</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>-0.0097</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>-0.0014</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="35">
@@ -1877,34 +1877,34 @@
         <v>-0.2567</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1063</v>
+        <v>-0.1501</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1288</v>
+        <v>-0.1215</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0037</v>
+        <v>-0.1209</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0037</v>
+        <v>-0.1195</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0036</v>
+        <v>-0.1177</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0036</v>
+        <v>-0.1162</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0929</v>
+        <v>-0.0255</v>
       </c>
       <c r="K35" t="n">
-        <v>0.1155</v>
+        <v>-0.0018</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>-0.0018</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>-0.0013</v>
       </c>
     </row>
     <row r="36">
@@ -2123,31 +2123,31 @@
         <v>-0.0061</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0008</v>
+        <v>-0.0047</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0001</v>
+        <v>0.001</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0001</v>
+        <v>0.0004</v>
       </c>
       <c r="G41" t="n">
-        <v>0.0015</v>
+        <v>0.0018</v>
       </c>
       <c r="H41" t="n">
+        <v>0.0026</v>
+      </c>
+      <c r="I41" t="n">
         <v>0.001</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0</v>
       </c>
       <c r="J41" t="n">
         <v>0.0002</v>
       </c>
       <c r="K41" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="L41" t="n">
         <v>0.001</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
       </c>
       <c r="M41" t="n">
         <v>0</v>
@@ -2164,34 +2164,34 @@
         <v>-0.2772</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1586</v>
+        <v>-0.0898</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1298</v>
+        <v>-0.0595</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0012</v>
+        <v>-0.0443</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.0783</v>
+        <v>-0.1286</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0049</v>
+        <v>-0.1382</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0038</v>
+        <v>-0.1339</v>
       </c>
       <c r="J42" t="n">
-        <v>0.0935</v>
+        <v>-0.0396</v>
       </c>
       <c r="K42" t="n">
-        <v>0.1201</v>
+        <v>-0.0072</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0002</v>
+        <v>-0.0023</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2410,31 +2410,31 @@
         <v>-0.0579</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0481</v>
+        <v>-0.0006</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>-0.0006</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="H48" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="K48" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="M48" t="n">
         <v>0</v>
@@ -2492,34 +2492,34 @@
         <v>0.0922</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.001</v>
+        <v>0.0911</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.001</v>
+        <v>0.0879</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.001</v>
+        <v>0.0192</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.085</v>
+        <v>-0.0664</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>-0.0632</v>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>-0.0619</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>0.0022</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>0.0032</v>
       </c>
       <c r="L50" t="n">
-        <v>0</v>
+        <v>-0.0007</v>
       </c>
       <c r="M50" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="51">
@@ -2533,31 +2533,31 @@
         <v>-0.0072</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0008</v>
+        <v>-0.0084</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0041</v>
+        <v>-0.0049</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0003</v>
+        <v>-0.0041</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0003</v>
+        <v>-0.004</v>
       </c>
       <c r="H51" t="n">
-        <v>0.0003</v>
+        <v>-0.004</v>
       </c>
       <c r="I51" t="n">
-        <v>0.0003</v>
+        <v>-0.0039</v>
       </c>
       <c r="J51" t="n">
-        <v>0.0003</v>
+        <v>-0.0039</v>
       </c>
       <c r="K51" t="n">
-        <v>0.0035</v>
+        <v>-0.0007</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="M51" t="n">
         <v>0</v>
@@ -2697,16 +2697,16 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="G55" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>

</xml_diff>